<commit_message>
feat(SPC_ONEDXINTERNAL-8888): Thêm tính năng tạo đề thi
</commit_message>
<xml_diff>
--- a/Câu hỏi Java.xlsx
+++ b/Câu hỏi Java.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="69">
   <si>
     <t>Câu hỏi</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Đáp án đúng</t>
   </si>
   <si>
-    <t>Đâu là câu SAI về ngôn ngữ Java?</t>
-  </si>
-  <si>
     <t>Ngôn ngữ Java có phân biệt chữ hoa – chữ thường</t>
   </si>
   <si>
@@ -52,13 +49,187 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>Đâu không phải là một kiểu dữ liệu nguyên thủy trong Java?</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>long float</t>
+  </si>
+  <si>
+    <t>Trong câu lệnh sau: public static void main(String[] agrs) thì phần tử agrs[0] chứa giá trị gì?</t>
+  </si>
+  <si>
+    <t>Tên của chương trình</t>
+  </si>
+  <si>
+    <t>Số lượng tham số</t>
+  </si>
+  <si>
+    <t>Không câu nào đúng</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Tham số đầu tiên trong danh sách tham số</t>
+  </si>
+  <si>
+    <t>Phương thức next() của lớp Scanner dùng để làm gì?</t>
+  </si>
+  <si>
+    <t>Nhập một số nguyên</t>
+  </si>
+  <si>
+    <t>Nhập một ký tự</t>
+  </si>
+  <si>
+    <t>Nhập một chuỗi</t>
+  </si>
+  <si>
+    <t>Không có phương thức này</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netbeans </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eclipse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JDK </t>
+  </si>
+  <si>
+    <t>Java Platform</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Đâu là khai báo đúng về lớp Cat?</t>
+  </si>
+  <si>
+    <t>interface Cat{}</t>
+  </si>
+  <si>
+    <t>public class Cat{}</t>
+  </si>
+  <si>
+    <t>static Cat{}</t>
+  </si>
+  <si>
+    <t>class public Cat{}</t>
+  </si>
+  <si>
+    <t>Gói nào trong java chứa lớp Scanner dùng để nhập dữ liệu từ bàn phím?</t>
+  </si>
+  <si>
+    <t> java.net</t>
+  </si>
+  <si>
+    <t>java.io</t>
+  </si>
+  <si>
+    <t>java.util</t>
+  </si>
+  <si>
+    <t>java.awt</t>
+  </si>
+  <si>
+    <t>Tên đầu tiên của Java là gì?</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Oak</t>
+  </si>
+  <si>
+    <t>Cafe</t>
+  </si>
+  <si>
+    <t>James golings</t>
+  </si>
+  <si>
+    <t>Giả sử đã định nghĩa lớp XX với một phương thức thông thường là Display, sau đó sinh ra đối tượng objX từ lớp XX. Để gọi phương thức Display ta sử dụng cú pháp nào?</t>
+  </si>
+  <si>
+    <t>Display();</t>
+  </si>
+  <si>
+    <t>objX.Display();</t>
+  </si>
+  <si>
+    <t>XX.Display();</t>
+  </si>
+  <si>
+    <t>XX.Display;</t>
+  </si>
+  <si>
+    <t>Tên lớp</t>
+  </si>
+  <si>
+    <t>Thuộc tính</t>
+  </si>
+  <si>
+    <t>Phương thức</t>
+  </si>
+  <si>
+    <t>Biến</t>
+  </si>
+  <si>
+    <t>Đối tượng trong Java là gì?</t>
+  </si>
+  <si>
+    <t>Đâu là câu sai về ngôn ngữ Java?</t>
+  </si>
+  <si>
+    <t>Muốn chạy được chương trình Java, chỉ cần cài phần mền nào sau đây?</t>
+  </si>
+  <si>
+    <t>Đâu không phải là thành phần trong cấu trúc của lớp trong Java.</t>
+  </si>
+  <si>
+    <t>Các lớp được tạo thể hiện từ đó</t>
+  </si>
+  <si>
+    <t>Một thể hiện của lớp</t>
+  </si>
+  <si>
+    <t>Một tham chiếu đến một thuộc tính</t>
+  </si>
+  <si>
+    <t>Một biến</t>
+  </si>
+  <si>
+    <t>Kiểu dữ liệu nào trong Java chứa giá trị bao gồm cả chữ và số?</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +246,12 @@
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF333333"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -99,10 +276,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,15 +582,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="123.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="51" style="1" customWidth="1"/>
     <col min="3" max="3" width="39.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="54.7109375" style="1" customWidth="1"/>
@@ -442,22 +620,242 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>